<commit_message>
correct Goldstein in Goldstein
</commit_message>
<xml_diff>
--- a/Cas test/Tests.xlsx
+++ b/Cas test/Tests.xlsx
@@ -59,12 +59,6 @@
     <t>Branin_2</t>
   </si>
   <si>
-    <t>Golstein_1</t>
-  </si>
-  <si>
-    <t>Golstein_2</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -171,6 +165,12 @@
   </si>
   <si>
     <t xml:space="preserve">Vanaret </t>
+  </si>
+  <si>
+    <t>Goldstein_1</t>
+  </si>
+  <si>
+    <t>Goldstein_2</t>
   </si>
 </sst>
 </file>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,7 +627,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -647,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>7</v>
@@ -664,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>7</v>
@@ -673,7 +673,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -682,7 +682,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>7</v>
@@ -690,7 +690,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -701,7 +701,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
@@ -710,16 +710,16 @@
         <v>0</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2">
         <v>10</v>
@@ -728,16 +728,16 @@
         <v>0</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -746,15 +746,15 @@
         <v>0</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -764,7 +764,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -773,7 +773,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>7</v>
@@ -782,7 +782,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -791,7 +791,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>7</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -810,7 +810,7 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2">
         <v>3</v>
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>7</v>
@@ -828,7 +828,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" s="2">
         <v>4</v>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>7</v>
@@ -846,7 +846,7 @@
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2">
         <v>2</v>
@@ -855,7 +855,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>7</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2">
         <v>7</v>
@@ -873,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>7</v>
@@ -881,7 +881,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
@@ -890,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>7</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -908,7 +908,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2">
         <v>1</v>
@@ -917,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>7</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -936,7 +936,7 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C23" s="2">
         <v>1</v>
@@ -945,7 +945,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>7</v>
@@ -954,7 +954,7 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="2">
         <v>1</v>
@@ -963,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>7</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C25" s="2">
         <v>2</v>
@@ -980,7 +980,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>7</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" s="2">
         <v>5</v>
@@ -997,7 +997,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>7</v>
@@ -1005,7 +1005,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C27" s="2">
         <v>2</v>
@@ -1014,7 +1014,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>7</v>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
@@ -1041,10 +1041,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>